<commit_message>
done with 512 testing
</commit_message>
<xml_diff>
--- a/evaluation/testing_results.xlsx
+++ b/evaluation/testing_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliki\Desktop\wiki_chatbot_ncpeh_ehealthlab\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A093DB96-9B96-41B9-884F-AF19F6412D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704E5AC0-8B25-43ED-8104-1D8F3159135A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="248">
   <si>
     <t>Question</t>
   </si>
@@ -690,6 +690,99 @@
   </si>
   <si>
     <t>Related_article</t>
+  </si>
+  <si>
+    <t>Answer_512</t>
+  </si>
+  <si>
+    <t>Evaluation_512</t>
+  </si>
+  <si>
+    <t>eDispensation is a service that allows citizens in Europe to retrieve their medication in a pharmacy located in another European country, thanks to the online transfer of their electronic prescription from their country of affiliation (hereafter referred to as the country of residence) to their country of travel. Your country of residence is informed about the medicine you retrieve in the country of travel (eDispensation). Currently the following 2 Electronic Cross-Border Health services are progressively introduced in all EU countries: ePrescription Patient Summaries provide information on important health related aspects such as allergies, current medication,previous illness, surgeries, etc. It is part of a larger collection of health data called an European Health Record whose implementation across Europe is planned at a later stage. The digital Patient Summary is meant to provide doctors with essential information in their own language concerning the patient, when the patient comes from another EU country and there may be a linguistic barrier. In the long term, medical images, lab results and hospital discharge reports will also be available across the EU, with the full health record to follow later on.</t>
+  </si>
+  <si>
+    <t>The Electronic Cross-Border Services in Europe will benefit European citizens in the following ways: 1. ePrescription: a.       It will be possible for European citizens to retrieve their medication in a pharmacy located in another European country, thanks to the online transfer of their electronic prescription from their country of affiliation (hereafter referred to as the country of residence) to their country of travel. b.   Their country of residence is informed about the medicine they retrieve in the country of travel (eDispensation). 2.        Patient Summary: a.     The Patient Summary provides information on important health related aspects such as allergies, current medication, previous illness, surgeries, etc. b.    It is part of a larger collection of health data called an European Health Record whose implementation across Europe is planned at a later stage. c.        The digital Patient Summary is meant to provide doctors with essential information in their own language concerning the patient, when the patient comes from another EU country and there may be a linguistic barrier. d.   In the long term, medical images, lab results and hospital discharge reports will also be available across the EU, with the full health record to follow later on..</t>
+  </si>
+  <si>
+    <t>The NCP eHealth(CY) Portal is a web-based application that allows healthcare professionals to access and manage patient data. The login process for the NCP eHealth(CY) Portal is as follows: 1. Go to the NCP eHealth(CY) Portal website (https://ncp.ehealth.gov.cy/) 2. Click on the "Login" button located in the top right corner of the page 3. Enter your username and password in the appropriate fields 4. Click on the "Login" button to access the NCP eHealth(CY) Portal 5. Once logged in, you will be able to access all the features and functions of the NCP eHealth(CY) Portal, including the ability to view patient data, create and manage patient records, and generate reports..</t>
+  </si>
+  <si>
+    <t>The NCP eHealth(Cyprus) Portal is a web-based application that provides a secure and convenient way for users to access and manage their healthcare information. The portal is divided into several modules, each with its own set of features and functions. The main module of the NCP eHealth(Cyprus) Portal is the Patient Module. This module allows patients to access their health records, view test results, schedule appointments, and communicate with their healthcare providers. Patients can also use the portal to pay their bills and view their insurance information. The Doctor Module is another important module of the NCP eHealth(Cyprus) Portal. This module allows doctors to access patient records, view test results, and communicate with their patients. Doctors can also use the portal to schedule appointments and view their billing information. The Pharmacy Module is another important module of the NCP eHealth(Cyprus) Portal. This module allows pharmacists to access patient records, view test results, and communicate with their patients. Pharmacists can also use the portal to view their billing information and manage their inventory. The NCP eHealth(Cyprus) Portal also includes a number of other modules, such as the Billing Module, the Inventory Module, and the Reporting Module. These modules allow users to manage their billing information, inventory, and reporting needs. Overall, the NCP eHealth(Cyprus) Portal provides users with a comprehensive set of features and functions that allow them to manage their healthcare information in a secure and convenient way..</t>
+  </si>
+  <si>
+    <t>The Patient Summary Report includes the following information: 1. Patient Identification 2. Patient Contact Information 3. Patient Insurance Information 4. Patient Clinical Data 5. Patient Medication Summary 6. Patient Allergies 7. Patient Surgical Procedures 8. Patient Current Problem/Diagnosis 9. Patient Medical Devices and Implants 10. Patient Treatment Recommendation 11. Patient Autonomy/Invalidity 12. Patient Social History 13. Patient Physical Findings 14. Patient Diagnostic Tests 15. Patient ePrescription</t>
+  </si>
+  <si>
+    <t>1. Search patient from Cyprus. 2. Provide CY national security number. 3. Retrieve Personal Details. 4. Retrieve PS list. 5. Open Clinical Document (translated XML document parsed in CDA Display Viewer)..</t>
+  </si>
+  <si>
+    <t>1. The doctor logs in to the portal. 2. The doctor selects the EU patient. 3. The doctor selects the country of origin of the EU patient. 4. The doctor selects the reason of accessing the patient data. 5. The doctor clicks on the “Retrieve Medical Documents List” button. 6. The doctor opens the PDF document. 7. The doctor opens the CDA Display Viewer. 8. The doctor selects the PS list. 9. The doctor selects the clinical document. 10. The doctor selects the language of the clinical document. 11. The doctor selects the country of origin of the clinical document. 12. The doctor selects the reason of accessing the clinical document. 13.</t>
+  </si>
+  <si>
+    <t>The clinical documents are displayed in the portal in the following way: 1. The patient’s personal details are displayed in the portal. 2</t>
+  </si>
+  <si>
+    <t>The pharmacist in the country of travel will be able to view on their computer the ePrescription prepared by the patient's doctor in their country of residence and provide the prescribed medicine. When citizens travel from their country of residence to another country in Europe and find themselves in the necessity of consulting a doctor in that country, doctors will be able to access the Patient Summary, which contains essential medical information related to the patient. This will help doctors to formulate an adequate treatment, avoid some possible risk (for instance in case of allergy) and overcome linguistic barriers. The Patient Summary will then be substituted at a later stage by the European Health Record which will contain more comprehensive health data. In order to enable the services to fully operate, citizens will be informed on whether their health data are available for cross-border services before travelling. In some countries citizens might be required to explicitly give their authorization in order to have their health data made available abroad. In any case, making health data available for cross-border exchange is needed in order for pharmacists and doctors to access it from the country where the patient travels. Adequate IT infrastructure has been put in place at European and national level to allow this smooth exchange of data. How does it Work? In electronic cross-border services your personal data will always be treated and protected in accordance with the existing EU legislation and with the current practices in your country of residence and the country of travel. In some, the cross-border exchange of your health data might be allowed by law and doesn't require any action from your part. In other countries of residence, on the contrary, you need to actively give your consent, meaning that you will have to sign a document (similar to a Privacy statement). Depending on your country, you can do this by contacting your doctor or electronically, by connecting to a specific website/web portal setup by your national authority. Please note that in case your consent is required and you don't give it in your country of residence before your departure or through mobile portal while travelling, it will not be possible for the pharmacist or the doctor in the country of destination to access your health data. In your you may also be asked to sign another document (similar to a Privacy statement) which allows the pharmacist or the doctor in that country to access your health</t>
+  </si>
+  <si>
+    <t>In the context of cross-border healthcare services, your personal data will always be treated and protected in accordance with the existing EU legislation and with the current practices in your country of residence and the country of travel. In some countries, the cross-border exchange of your health data might be allowed by law and doesn’t require any action from your part. In other countries of residence, on the contrary, you need to actively give your consent, meaning that you will have to sign a document (similar to a Privacy statement). Depending on your country, you can do this by contacting your doctor or electronically, by connecting to a specific website/web portal setup by your national authority. Please note that in case your consent is required and you don’t give it in your country of residence before your departure or through mobile portal while travelling, it will not be possible for the pharmacist or the doctor in the country of destination to access your health data. In your country of residence, you may also be asked to sign another document (similar to a Privacy statement) which allows the pharmacist or the doctor in that country to access your health data. It is important to know that your health data are being exchanged through a secured communication channel and can only be accessed by health professionals (doctors or pharmacists) who are clearly and securely identified and authorized to access your health data. High security measures are in place in order to make sure that your health data cannot be accessed by unauthorized persons..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The European Health Insurance Card (EHIC) is a document that gives you the right to access state-provided healthcare during a temporary stay in another EU country. It is not an alternative to having your own personal health insurance. The EHIC is not a substitute for travel insurance. It does not cover medical repatriation, ongoing medical treatment or non-urgent medical attention. The EHIC is not valid for medical repatriation, ongoing medical treatment or non-urgent medical attention. </t>
+  </si>
+  <si>
+    <t>Depending on the member state, you may be required, before your departure,to check via your doctor or your national patients’ portal if your health data are automatically available for electronic cross-border services or if you need to give your consent for that. If you have online access to your health data, please pay attention to the instructions you receive on how to give your consent electronically. Make sure you have a document to clearly identify yourself (see question below) If needed, give consent to allow the pharmacist/doctor to access your health data. Do I have access to the same health services in my country of travel as the citizens living there? As an EU citizen, if you unexpectedly fall ill during atemporary stay abroad, you are entitled to any treatment that can't wait until you get home. You have the same rights to healthcare as people insured in the country you are in. It is advisable to take your European Health Insurance Card (EHIC) with you on all trips abroad This card is the physical proof that you are insured in an EU country and will simplify payment and reimbursement procedures.However,if you don't have your card or if it is not possible to use it, you may not be refused treatment. You may, however, have to pay for it upfront and claim reimbursement once backhome. I don't speak the pharmacist's language. How will the pharmacist get the right information from my doctor? The pharmacists in your country of travel will get your ePrescription in their own language,together with an original copyof your ePrescriptionwhich is in yourlanguage.So,theprescription originally done by your doctor will be available in the pharmacist's system in both languages. How will I know how to take the medication? The terms of use of your medicine (package leaflet) will be available in the language(s) of the country of travel and might be also available in other languages. Concerning the patient-specific guidance, it will be available in your own language and the pharmacist will explain to you in the best possible way how to take your medicine. What document do I need to take with me when going to a Pharmacy or consulting a doctor abroad? When requesting your medicine in a pharmacy in the country of travel or</t>
+  </si>
+  <si>
+    <t>The pharmacists in your country of travel will get your ePrescription in their own language, together with an original copy of your ePrescription which is in your language. So, the prescription originally done by your doctor will be available in the pharmacist's system in both languages.</t>
+  </si>
+  <si>
+    <t>When requesting your medicine in a pharmacy in the country of travel or if you consult a doctor there, you will need to clearly identify yourself. Each country has defined the type of identification document that the patient has to show to identify themselves when using the ePrescription. You need to check with your own national contact point for eHealth what identification document you need. Unfortunately, there is no absolute certainty that a specific prescription can be dispensed. The supply of medicines at a pharmacy in your country of travel may be more limited than in your country of residence, the pharmacy may not stock the medicine, and there is no available substitution. Furthermore, the medicine in question may not have a marketing authorisation in the country of travel. The pharmacist may also refuse to dispense a medication due to the substitution rules for medicinal products in the country of travel. A pharmacy dispenses the medication according to the legislation in its country. My prescription is quite ordinary.</t>
+  </si>
+  <si>
+    <t>The National eHealth Authority (NeHA) is the competent authority for the implementation of the eHealth Strategy in Cyprus. The NeHA is responsible for the development and implementation of the National eHealth Strategy and the National eHealth Action Plan. The NeHA is also responsible for the development and implementation of the National eHealth Portal. The National eHealth Portal is the main tool for the implementation of the eHealth Strategy in Cyprus. The National eHealth Portal is a centralized platform that provides access to eHealth services and information for citizens, healthcare professionals, and healthcare organizations. The National eHealth Portal is a one-stop shop for all eHealth services and information in Cyprus. The National eHealth Portal provides access to a wide range of eHealth services and information, including: - Electronic Health Records (EHRs) - Electronic Prescriptions (ePrescriptions) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (EHRs) - Electronic Health Records (E</t>
+  </si>
+  <si>
+    <t>The Patient Summary can contain the following patient clinical data: - Alerts and allergies; - Medical history (vaccination, past problems, surgical procedures before the last six months); - Current medical state (current problems, medical devices and implants, intake of medicines, treatment recommendations, surgical procedures within the last six months); - Social history; - Pregnancy history (if relevant); - Physical findings; - Diagnostic tests. It is not mandatory that all this information exists. This means that there might be situations when only part of the information is available. For instance when the information was not available in the systems; the information could not be translated into other languages; there is no known information for that patient; etc. Refer to the training provided by your national contact point for eHealth on how to read the information in the Patient Summary. If you have not received any training, please contact your National eHealth Authority.</t>
+  </si>
+  <si>
+    <t>You are an expert in answering questions related to the Deployment of Generic Cross Border eHealth in Cyprus. Given a question and relevant information from the article 'NCP eHealth(Cyprus) Portal - Information for the Patient Page 9 National eHealth Authority - Cyprus Please request a prescription from a doctor in the country of travel. No, such a prescription cannot be dispensed in your country of residence using the cross border electronic services. In case you received a paper copy of your prescription and provided the prescription includes the required information, the pharmacy from your country of residence should dispense your prescription. For acting on behalf of someone else, you must follow the applicable provisions of each country. This first depends on the national provisions implementing data protection legislation in each country, but also, depending on the country and your needs, you might be asked to provide additional documents as proof of authority to act on behalf of another person (e.g. proof of your identity, birth certificate if you are acting on behalf of a minor, power of attorney). Please consider there might be countries which do not allow acting on behalf of someone else in such situations. I was unable to obtain medicine from a pharmacy in my country of travel, but I need it urgently. What shall I do? I am a European citizen who travelled to another European country and had an electronic prescription issued in the country of travel. Can I retrieve the prescribed medicine from my country of residence? Can I purchase medicines on behalf of someone else, for instance my child or my wife? NCP eHealth(CY) Portal - Doctors in the Country of Residence Page 10 National eHealth Authority - Cyprus Does every doctor in the country of travel automatically have access to the patient's health data? Do I need to indicate or inform that my patient is travelling? Authorized doctors and pharmacists, according to the legislation in the countries of travel, can have access to the patient's health data only if the patient's health data is available for electronic cross border services. In some countries of residence, citizens are required to explicitly give their consent, whereas in other countries of residence, the electronic cross-border exchange of patient's health data might be allowed by law and does not require any action from the patient's part. In any case</t>
+  </si>
+  <si>
+    <t>No, such a prescription cannot be dispensed in your country of residence using the cross border electronic services. In case you received a paper copy of your prescription and provided the prescription includes the required information, the pharmacy from your country of residence should dispense your prescription. For acting on behalf of someone else, you must follow the applicable provisions of each country. This first depends on the national provisions implementing data protection legislation in each country, but also, depending on the country and your needs, you might be asked to provide additional documents as proof of authority to act on behalf of another person (e.g. proof of your identity, birth certificate if you are acting on behalf of a minor, power of attorney). Please consider there might be countries which do not allow acting on behalf of someone else in such situations. I was unable to obtain medicine from a pharmacy in my country of travel, but I need it urgently.</t>
+  </si>
+  <si>
+    <t>Authorized doctors and pharmacists, according to the legislation in the countries of travel, can have access to the patient's health data only if the patient's health data is available for electronic cross border services. In some countries of residence, citizens are required to explicitly give their consent, whereas in other countries of residence, the electronic cross-border exchange of patient's health data might be allowed by law and does not require any action from the patient's part. In any case, pharmacists and doctors in the country of treatment can only access health data if it has been made available for electronic cross-border exchange by the country of residence. In addition, in some countries of travel, doctors and pharmacists may have to ask the foreign patient to sign an additional Privacy statement, to enable them to comply with the law in their country and to be able to process patient's data. Doctors in the country of residence. Depending on the MemberState, you should inform your patients about the possibility of making their health data available for electronic cross-border services when travelling, either through your own support or by accessing a national portal. It is not necessary to indicate if thepatient will travel. National portals are different for each Member State; please check this accordingly,by referring to the information provided by your national contact point for eHealth on how to communicate about the availability of the electronic cross-border services. If you have not received any training, please contact your national contact point for eHealth. NCP eHealth(CY) Portal - Doctors in the Country of Residence Page 12 National eHealth Authority - Cyprus</t>
+  </si>
+  <si>
+    <t>You are an expert in answering questions related to the Deployment of Generic Cross Border eHealth in Cyprus. Given a question and relevant information from the article 'NCP eHealth(CY) Portal - Doctors in the Country of Residence Page 12 National eHealth Authority - Cyprus You will write your ePrescription in your own language. When the patient will ask for medicines in the country of travel, the pharmacist will receive thee Prescription both in theoriginal languageand in their own language. Translation is done automatically by the underlying digital infrastructure.</t>
+  </si>
+  <si>
+    <t>The Patient Summary can contain the following patient clinical data: - Alerts and allergies; - Medical history (vaccination, past problems, surgical procedures before the last six months); - Current medical state (current problems, medical devices and implants, intake of medicines, treatment recommendations, surgical procedures within the last six months); - Social history; - Pregnancy history (if relevant); - Physical findings; - Diagnostic tests. It is not mandatory that all this information exists. This means that there might be situations when only part of the information is available. For instance when the information was not available in the systems; the information could not be translated into other languages; there is no known information for that patient; etc. Refer to the training provided by your national contact point for eHealth on how to read the information in the Patient Summary. If you have not received any training, please contact your national contact point for eHealth.</t>
+  </si>
+  <si>
+    <t>Two Factor Authentication (2FA) is a security feature that requires two different methods of authentication to verify your identity. This can be done with a password and a code sent to your phone, or with a physical token like a key fob or a card..</t>
+  </si>
+  <si>
+    <t>The NCP eHealth(CY) Portal is a crucial component of the NCP eHealth(CY) framework, which aims to facilitate secure cross-border healthcare services in Cyprus. The portal is managed by the National eHealth Authority (NeHA), which is responsible for creating and managing user roles and access levels. The portal is designed to facilitate secure communication between healthcare professionals and pharmacies, and to ensure the integrity of sensitive healthcare data. The portal is managed by a team of NeHA Administrators, who are responsible for creating and managing user roles and access levels. The Administrators work closely with Operators, who are responsible for managing the day-to-day operations of the portal. The Administrators and Operators collaborate to ensure that the portal is secure and that healthcare professionals and pharmacies have the appropriate access levels to perform their duties. The Administrators and Operators work together to ensure that the portal is secure and that healthcare professionals and pharmacies have the appropriate access levels to perform their duties. The Administrators create and manage user roles and access levels, while the Operators manage the day-to-day operations of the portal</t>
+  </si>
+  <si>
+    <t>The MyHealth@EU Service is depicted in the graphical flow diagram as a centralized system that facilitates the secure exchange of healthcare data between healthcare providers and patients. The system is designed to ensure the privacy and security of patient data, with a focus on cross-border services. The graphical flow diagram depicts the various roles and responsibilities involved in the system, including the National eHealth Authority, healthcare providers, and patients. The diagram also highlights the various steps involved in the exchange of healthcare data, including the creation of a secure connection, the exchange of data, and the verification of the data. The diagram also highlights the various security measures in place to protect patient data, including encryption and authentication..</t>
+  </si>
+  <si>
+    <t>The NCPeH CY framework in Cyprus represents a crucial advancement in safeguarding healthcare data and ensuring patient privacy and security. At the heart of this system lies a network of roles and responsibilities designed to uphold the integrity of sensitive information and facilitate secure cross-border services. The following subsections outline the key roles and corresponding responsibilities. within the NCPeH CY framework, elucidating the collaborative efforts required to fortify the healthcare ecosystem against cyber threats and privacy breaches. Roles and responsibilities of the National Registry Portal Introduction - NCP Registry Roles NCP eHealth(Cyprus) Portal - Registry Roles Page 25 National eHealth Authority - Cyprus Role Administrator - NeHA The Administrator NeHA is a central figure in the management of the healthcare administration system NCPeH CY.This role is endowed with creating new users a level of access and control, primarily focusing on the access control and management of the system. Responsibilities Adding New Roles: The Administrator NeHA is responsible for creating new roles within the system to accommodate evolving administrative needs. This includes the crucial role of the Operator -NeHA, which plays a significant part in managing pharmacists and pharmacies. Role NeHA Operator Notice The NCPeHealth(CY) Roles Described in this section are to be managed by the Officers of The National eHealth Authority of Cyprus under agreed governance with the Cyprus Medical Association and Cyprus Pharmaceutical Association respectively. NCP eHealth(Cyprus) Portal - Registry Roles Page 26 National eHealth Authority - Cyprus The NeHa Operator role is pivotal in managing the system's day-to-day operations, with a focus on pharmacists, pharmacies, and certification processes. : Viewing all pharmacists, physicians, and pharmacies within the system. The ability to edit details of pharmacists and pharmacies to ensure up-to-date and accurate information. : Empowered to enable or disable pharmacists and physicians within the system, ensuring only authorized individuals have access. Viewing active, exp</t>
+  </si>
+  <si>
+    <t>The graphical flow of the MyHealth@EU Service is a visual representation of the steps involved in the process of exchanging health data between different healthcare providers in the European Union. The graphical flow consists of several stages or components, each with a specific purpose and function. The first stage is the registration of healthcare providers. This stage involves the creation of a profile for each healthcare provider, including their name, address, and other relevant information. This information is used to identify the healthcare provider and to ensure that they are authorized to participate in the exchange of health data. The second stage is the creation of a patient profile. This stage involves the creation of a profile for each patient, including their name, address, and other relevant information. This information is used to identify the patient and to ensure that they are authorized to participate in the exchange of health data. The third stage is the creation of a health data exchange agreement. This stage involves the creation of an agreement between the healthcare provider and the patient, outlining the terms and conditions for the exchange of health data. This agreement is used to ensure that both parties understand the terms and conditions of the exchange and that they are in compliance with applicable laws and regulations. The fourth stage is the exchange of health data. This stage involves the actual exchange of health data between the healthcare provider and the patient. This exchange is facilitated by the use of secure communication channels and encryption technologies to ensure the confidentiality and security of the data. The fifth stage is the verification of health data. This stage involves the verification of the health data exchanged between the healthcare provider and the patient. This verification is performed to ensure that the data is accurate and complete and that it meets the requirements of the health data exchange agreement. The sixth stage is the storage of health data. This stage involves the storage of the health data exchanged between the healthcare provider and the patient. This storage is performed to ensure that the data is available for future use and that it can be accessed by authorized healthcare providers. The seventh stage is the analysis of health data. This stage involves the analysis of the health data exchanged between the healthcare provider and the patient. This analysis is performed to identify trends and patterns in the data and to identify potential health risks. The eighth stage is the reporting of health data. This stage involves the reporting of the health</t>
+  </si>
+  <si>
+    <t>Certificates play a crucial role in the roles of pharmacists and physicians within the system. They are used to verify and authenticate professional qualifications and services, ensuring that only qualified and authorized individuals can access and use the system. Certificates are created and managed by pharmacists and physicians, who are responsible for ensuring that the information contained in the certificates is accurate and up-to-date. This includes information such as the individual's name, qualifications, and any restrictions or limitations on their practice. Certificates are also used to verify the authenticity of professional qualifications and services. For example, a pharmacist may use a certificate to verify the qualifications of a physician before prescribing a medication. Similarly, a physician may use a certificate to verify the qualifications of a pharmacist before dispensing a prescription. In summary, certificates are an essential tool for ensuring the quality and safety of healthcare services in the system. They provide a secure and reliable way to verify and authenticate professional qualifications and services, ensuring that only qualified and authorized individuals can access and use the system..</t>
+  </si>
+  <si>
+    <t>The responsibilities associated with the creation of certificates for physicians and pharmacists are as follows: Physicians: - Create new certificates for themselves and other professionals. - View their active, revoked, and expired certificates. - Revocate active certificates. Pharmacists: - Create new certificates for themselves and other professionals.</t>
+  </si>
+  <si>
+    <t>The NCP eHealth(Cyprus) Portal is a digital platform that provides a secure and efficient way for healthcare professionals to share and access patient information. The portal is designed to facilitate cross-border eHealth services, allowing healthcare providers to collaborate and coordinate care for patients who may be receiving treatment in multiple countries. The portal is managed by the National eHealth Authority (NeHA) in Cyprus, which is responsible for the development and implementation of the portal. The NeHA is a government agency that is tasked with promoting the use of eHealth technologies in the healthcare sector. The portal is designed to be user-friendly and accessible to healthcare professionals from all over the world. It provides a secure and encrypted environment for healthcare providers to share patient information, including medical records, test results, and other relevant data. The portal is also designed to be compliant with international standards and regulations, ensuring that patient data is protected and secure. This includes measures such as encryption, authentication, and access control, which help to prevent unauthorized access to patient information. The portal is also designed to be scalable, allowing it to accommodate the needs of healthcare providers from different countries and regions. This means that the portal can be adapted to meet the specific needs of different healthcare systems, ensuring that it remains relevant and useful for healthcare providers around the world. Overall, the NCP eHealth(Cyprus) Portal is a valuable tool for healthcare providers who are looking to improve the quality of care for their patients. It provides a secure and efficient way for healthcare professionals to share and access patient information, while also ensuring that patient data is protected and secure..</t>
   </si>
 </sst>
 </file>
@@ -1007,11 +1100,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,10 +1114,12 @@
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1041,10 +1136,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1060,11 +1161,17 @@
       <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1080,11 +1187,17 @@
       <c r="E3" t="s">
         <v>89</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1100,11 +1213,17 @@
       <c r="E4" t="s">
         <v>89</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1120,11 +1239,17 @@
       <c r="E5" t="s">
         <v>89</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1140,11 +1265,17 @@
       <c r="E6" t="s">
         <v>90</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1160,11 +1291,17 @@
       <c r="E7" t="s">
         <v>89</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1180,11 +1317,17 @@
       <c r="E8" t="s">
         <v>89</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1200,11 +1343,17 @@
       <c r="E9" t="s">
         <v>89</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1220,11 +1369,17 @@
       <c r="E10" t="s">
         <v>91</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="s">
+        <v>220</v>
+      </c>
+      <c r="G10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1240,11 +1395,17 @@
       <c r="E11" t="s">
         <v>89</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1260,11 +1421,17 @@
       <c r="E12" t="s">
         <v>89</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1280,11 +1447,17 @@
       <c r="E13" t="s">
         <v>89</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="s">
+        <v>221</v>
+      </c>
+      <c r="G13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1300,11 +1473,17 @@
       <c r="E14" t="s">
         <v>91</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="s">
+        <v>222</v>
+      </c>
+      <c r="G14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1320,11 +1499,17 @@
       <c r="E15" t="s">
         <v>91</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1340,11 +1525,17 @@
       <c r="E16" t="s">
         <v>89</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="s">
+        <v>223</v>
+      </c>
+      <c r="G16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1360,11 +1551,17 @@
       <c r="E17" t="s">
         <v>89</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>224</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1380,11 +1577,17 @@
       <c r="E18" t="s">
         <v>91</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="s">
+        <v>225</v>
+      </c>
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1400,11 +1603,17 @@
       <c r="E19" t="s">
         <v>89</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1420,11 +1629,17 @@
       <c r="E20" t="s">
         <v>90</v>
       </c>
-      <c r="F20">
+      <c r="F20" t="s">
+        <v>226</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1440,11 +1655,17 @@
       <c r="E21" t="s">
         <v>91</v>
       </c>
-      <c r="F21">
+      <c r="F21" t="s">
+        <v>227</v>
+      </c>
+      <c r="G21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1460,11 +1681,17 @@
       <c r="E22" t="s">
         <v>89</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1480,11 +1707,17 @@
       <c r="E23" t="s">
         <v>90</v>
       </c>
-      <c r="F23">
+      <c r="F23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1500,11 +1733,17 @@
       <c r="E24" t="s">
         <v>89</v>
       </c>
-      <c r="F24">
+      <c r="F24" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1520,11 +1759,17 @@
       <c r="E25" t="s">
         <v>91</v>
       </c>
-      <c r="F25">
+      <c r="F25" t="s">
+        <v>228</v>
+      </c>
+      <c r="G25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1540,11 +1785,17 @@
       <c r="E26" t="s">
         <v>90</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1560,11 +1811,17 @@
       <c r="E27" t="s">
         <v>89</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="s">
+        <v>188</v>
+      </c>
+      <c r="G27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1580,11 +1837,17 @@
       <c r="E28" t="s">
         <v>89</v>
       </c>
-      <c r="F28">
+      <c r="F28" t="s">
+        <v>229</v>
+      </c>
+      <c r="G28" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1600,11 +1863,17 @@
       <c r="E29" t="s">
         <v>89</v>
       </c>
-      <c r="F29">
+      <c r="F29" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1620,11 +1889,17 @@
       <c r="E30" t="s">
         <v>89</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1640,11 +1915,17 @@
       <c r="E31" t="s">
         <v>90</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="s">
+        <v>230</v>
+      </c>
+      <c r="G31" t="s">
+        <v>91</v>
+      </c>
+      <c r="H31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1660,11 +1941,17 @@
       <c r="E32" t="s">
         <v>89</v>
       </c>
-      <c r="F32">
+      <c r="F32" t="s">
+        <v>122</v>
+      </c>
+      <c r="G32" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1680,11 +1967,17 @@
       <c r="E33" t="s">
         <v>89</v>
       </c>
-      <c r="F33">
+      <c r="F33" t="s">
+        <v>191</v>
+      </c>
+      <c r="G33" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1700,11 +1993,17 @@
       <c r="E34" t="s">
         <v>91</v>
       </c>
-      <c r="F34">
+      <c r="F34" t="s">
+        <v>231</v>
+      </c>
+      <c r="G34" t="s">
+        <v>89</v>
+      </c>
+      <c r="H34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1720,11 +2019,17 @@
       <c r="E35" t="s">
         <v>89</v>
       </c>
-      <c r="F35">
+      <c r="F35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G35" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1740,11 +2045,17 @@
       <c r="E36" t="s">
         <v>91</v>
       </c>
-      <c r="F36">
+      <c r="F36" t="s">
+        <v>232</v>
+      </c>
+      <c r="G36" t="s">
+        <v>89</v>
+      </c>
+      <c r="H36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1760,11 +2071,17 @@
       <c r="E37" t="s">
         <v>89</v>
       </c>
-      <c r="F37">
+      <c r="F37" t="s">
+        <v>194</v>
+      </c>
+      <c r="G37" t="s">
+        <v>89</v>
+      </c>
+      <c r="H37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1780,11 +2097,17 @@
       <c r="E38" t="s">
         <v>89</v>
       </c>
-      <c r="F38">
+      <c r="F38" t="s">
+        <v>128</v>
+      </c>
+      <c r="G38" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1800,11 +2123,17 @@
       <c r="E39" t="s">
         <v>89</v>
       </c>
-      <c r="F39">
+      <c r="F39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G39" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1820,11 +2149,17 @@
       <c r="E40" t="s">
         <v>89</v>
       </c>
-      <c r="F40">
+      <c r="F40" t="s">
+        <v>195</v>
+      </c>
+      <c r="G40" t="s">
+        <v>89</v>
+      </c>
+      <c r="H40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1840,11 +2175,17 @@
       <c r="E41" t="s">
         <v>89</v>
       </c>
-      <c r="F41">
+      <c r="F41" t="s">
+        <v>196</v>
+      </c>
+      <c r="G41" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1860,11 +2201,17 @@
       <c r="E42" t="s">
         <v>89</v>
       </c>
-      <c r="F42">
+      <c r="F42" t="s">
+        <v>132</v>
+      </c>
+      <c r="G42" t="s">
+        <v>89</v>
+      </c>
+      <c r="H42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1880,11 +2227,17 @@
       <c r="E43" t="s">
         <v>89</v>
       </c>
-      <c r="F43">
+      <c r="F43" t="s">
+        <v>198</v>
+      </c>
+      <c r="G43" t="s">
+        <v>89</v>
+      </c>
+      <c r="H43">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1900,11 +2253,17 @@
       <c r="E44" t="s">
         <v>90</v>
       </c>
-      <c r="F44">
+      <c r="F44" t="s">
+        <v>233</v>
+      </c>
+      <c r="G44" t="s">
+        <v>90</v>
+      </c>
+      <c r="H44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1920,11 +2279,17 @@
       <c r="E45" t="s">
         <v>90</v>
       </c>
-      <c r="F45">
+      <c r="F45" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" t="s">
+        <v>89</v>
+      </c>
+      <c r="H45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1940,11 +2305,17 @@
       <c r="E46" t="s">
         <v>89</v>
       </c>
-      <c r="F46">
+      <c r="F46" t="s">
+        <v>135</v>
+      </c>
+      <c r="G46" t="s">
+        <v>89</v>
+      </c>
+      <c r="H46">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1960,11 +2331,17 @@
       <c r="E47" t="s">
         <v>89</v>
       </c>
-      <c r="F47">
+      <c r="F47" t="s">
+        <v>136</v>
+      </c>
+      <c r="G47" t="s">
+        <v>89</v>
+      </c>
+      <c r="H47">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1980,11 +2357,17 @@
       <c r="E48" t="s">
         <v>90</v>
       </c>
-      <c r="F48">
+      <c r="F48" t="s">
+        <v>235</v>
+      </c>
+      <c r="G48" t="s">
+        <v>90</v>
+      </c>
+      <c r="H48">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2000,11 +2383,17 @@
       <c r="E49" t="s">
         <v>90</v>
       </c>
-      <c r="F49">
+      <c r="F49" t="s">
+        <v>236</v>
+      </c>
+      <c r="G49" t="s">
+        <v>89</v>
+      </c>
+      <c r="H49">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -2020,11 +2409,17 @@
       <c r="E50" t="s">
         <v>90</v>
       </c>
-      <c r="F50">
+      <c r="F50" t="s">
+        <v>237</v>
+      </c>
+      <c r="G50" t="s">
+        <v>89</v>
+      </c>
+      <c r="H50">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -2040,11 +2435,17 @@
       <c r="E51" t="s">
         <v>90</v>
       </c>
-      <c r="F51">
+      <c r="F51" t="s">
+        <v>238</v>
+      </c>
+      <c r="G51" t="s">
+        <v>90</v>
+      </c>
+      <c r="H51">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -2060,11 +2461,17 @@
       <c r="E52" t="s">
         <v>90</v>
       </c>
-      <c r="F52">
+      <c r="F52" t="s">
+        <v>239</v>
+      </c>
+      <c r="G52" t="s">
+        <v>89</v>
+      </c>
+      <c r="H52">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2080,11 +2487,17 @@
       <c r="E53" t="s">
         <v>89</v>
       </c>
-      <c r="F53">
+      <c r="F53" t="s">
+        <v>205</v>
+      </c>
+      <c r="G53" t="s">
+        <v>89</v>
+      </c>
+      <c r="H53">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -2100,11 +2513,17 @@
       <c r="E54" t="s">
         <v>90</v>
       </c>
-      <c r="F54">
+      <c r="F54" t="s">
+        <v>238</v>
+      </c>
+      <c r="G54" t="s">
+        <v>90</v>
+      </c>
+      <c r="H54">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -2120,11 +2539,17 @@
       <c r="E55" t="s">
         <v>89</v>
       </c>
-      <c r="F55">
+      <c r="F55" t="s">
+        <v>142</v>
+      </c>
+      <c r="G55" t="s">
+        <v>89</v>
+      </c>
+      <c r="H55">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -2140,11 +2565,17 @@
       <c r="E56" t="s">
         <v>89</v>
       </c>
-      <c r="F56">
+      <c r="F56" t="s">
+        <v>143</v>
+      </c>
+      <c r="G56" t="s">
+        <v>89</v>
+      </c>
+      <c r="H56">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -2160,11 +2591,17 @@
       <c r="E57" t="s">
         <v>89</v>
       </c>
-      <c r="F57">
+      <c r="F57" t="s">
+        <v>144</v>
+      </c>
+      <c r="G57" t="s">
+        <v>89</v>
+      </c>
+      <c r="H57">
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -2180,11 +2617,17 @@
       <c r="E58" t="s">
         <v>89</v>
       </c>
-      <c r="F58">
+      <c r="F58" t="s">
+        <v>206</v>
+      </c>
+      <c r="G58" t="s">
+        <v>89</v>
+      </c>
+      <c r="H58">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -2200,11 +2643,17 @@
       <c r="E59" t="s">
         <v>89</v>
       </c>
-      <c r="F59">
+      <c r="F59" t="s">
+        <v>146</v>
+      </c>
+      <c r="G59" t="s">
+        <v>89</v>
+      </c>
+      <c r="H59">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -2220,11 +2669,17 @@
       <c r="E60" t="s">
         <v>89</v>
       </c>
-      <c r="F60">
+      <c r="F60" t="s">
+        <v>147</v>
+      </c>
+      <c r="G60" t="s">
+        <v>89</v>
+      </c>
+      <c r="H60">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -2240,11 +2695,17 @@
       <c r="E61" t="s">
         <v>89</v>
       </c>
-      <c r="F61">
+      <c r="F61" t="s">
+        <v>206</v>
+      </c>
+      <c r="G61" t="s">
+        <v>89</v>
+      </c>
+      <c r="H61">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -2260,11 +2721,17 @@
       <c r="E62" t="s">
         <v>89</v>
       </c>
-      <c r="F62">
+      <c r="F62" t="s">
+        <v>149</v>
+      </c>
+      <c r="G62" t="s">
+        <v>89</v>
+      </c>
+      <c r="H62">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -2280,11 +2747,17 @@
       <c r="E63" t="s">
         <v>89</v>
       </c>
-      <c r="F63">
+      <c r="F63" t="s">
+        <v>150</v>
+      </c>
+      <c r="G63" t="s">
+        <v>89</v>
+      </c>
+      <c r="H63">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -2300,11 +2773,17 @@
       <c r="E64" t="s">
         <v>90</v>
       </c>
-      <c r="F64">
+      <c r="F64" t="s">
+        <v>146</v>
+      </c>
+      <c r="G64" t="s">
+        <v>89</v>
+      </c>
+      <c r="H64">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -2320,11 +2799,17 @@
       <c r="E65" t="s">
         <v>89</v>
       </c>
-      <c r="F65">
+      <c r="F65" t="s">
+        <v>146</v>
+      </c>
+      <c r="G65" t="s">
+        <v>89</v>
+      </c>
+      <c r="H65">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -2340,11 +2825,17 @@
       <c r="E66" t="s">
         <v>89</v>
       </c>
-      <c r="F66">
+      <c r="F66" t="s">
+        <v>151</v>
+      </c>
+      <c r="G66" t="s">
+        <v>89</v>
+      </c>
+      <c r="H66">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -2360,11 +2851,17 @@
       <c r="E67" t="s">
         <v>89</v>
       </c>
-      <c r="F67">
+      <c r="F67" t="s">
+        <v>152</v>
+      </c>
+      <c r="G67" t="s">
+        <v>89</v>
+      </c>
+      <c r="H67">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -2380,11 +2877,17 @@
       <c r="E68" t="s">
         <v>89</v>
       </c>
-      <c r="F68">
+      <c r="F68" t="s">
+        <v>151</v>
+      </c>
+      <c r="G68" t="s">
+        <v>89</v>
+      </c>
+      <c r="H68">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -2400,11 +2903,17 @@
       <c r="E69" t="s">
         <v>89</v>
       </c>
-      <c r="F69">
+      <c r="F69" t="s">
+        <v>153</v>
+      </c>
+      <c r="G69" t="s">
+        <v>89</v>
+      </c>
+      <c r="H69">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -2420,11 +2929,17 @@
       <c r="E70" t="s">
         <v>89</v>
       </c>
-      <c r="F70">
+      <c r="F70" t="s">
+        <v>240</v>
+      </c>
+      <c r="G70" t="s">
+        <v>89</v>
+      </c>
+      <c r="H70">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -2440,11 +2955,17 @@
       <c r="E71" t="s">
         <v>91</v>
       </c>
-      <c r="F71">
+      <c r="F71" t="s">
+        <v>241</v>
+      </c>
+      <c r="G71" t="s">
+        <v>89</v>
+      </c>
+      <c r="H71">
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -2460,11 +2981,17 @@
       <c r="E72" t="s">
         <v>89</v>
       </c>
-      <c r="F72">
+      <c r="F72" t="s">
+        <v>242</v>
+      </c>
+      <c r="G72" t="s">
+        <v>89</v>
+      </c>
+      <c r="H72">
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -2480,11 +3007,17 @@
       <c r="E73" t="s">
         <v>91</v>
       </c>
-      <c r="F73">
+      <c r="F73" t="s">
+        <v>243</v>
+      </c>
+      <c r="G73" t="s">
+        <v>90</v>
+      </c>
+      <c r="H73">
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -2500,11 +3033,17 @@
       <c r="E74" t="s">
         <v>91</v>
       </c>
-      <c r="F74">
+      <c r="F74" t="s">
+        <v>244</v>
+      </c>
+      <c r="G74" t="s">
+        <v>90</v>
+      </c>
+      <c r="H74">
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -2520,11 +3059,17 @@
       <c r="E75" t="s">
         <v>89</v>
       </c>
-      <c r="F75">
+      <c r="F75" t="s">
+        <v>159</v>
+      </c>
+      <c r="G75" t="s">
+        <v>89</v>
+      </c>
+      <c r="H75">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -2540,11 +3085,17 @@
       <c r="E76" t="s">
         <v>89</v>
       </c>
-      <c r="F76">
+      <c r="F76" t="s">
+        <v>211</v>
+      </c>
+      <c r="G76" t="s">
+        <v>89</v>
+      </c>
+      <c r="H76">
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2560,11 +3111,17 @@
       <c r="E77" t="s">
         <v>89</v>
       </c>
-      <c r="F77">
+      <c r="F77" t="s">
+        <v>161</v>
+      </c>
+      <c r="G77" t="s">
+        <v>89</v>
+      </c>
+      <c r="H77">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>81</v>
       </c>
@@ -2580,11 +3137,17 @@
       <c r="E78" t="s">
         <v>91</v>
       </c>
-      <c r="F78">
+      <c r="F78" t="s">
+        <v>212</v>
+      </c>
+      <c r="G78" t="s">
+        <v>89</v>
+      </c>
+      <c r="H78">
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -2600,11 +3163,17 @@
       <c r="E79" t="s">
         <v>89</v>
       </c>
-      <c r="F79">
+      <c r="F79" t="s">
+        <v>163</v>
+      </c>
+      <c r="G79" t="s">
+        <v>89</v>
+      </c>
+      <c r="H79">
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>83</v>
       </c>
@@ -2620,11 +3189,17 @@
       <c r="E80" t="s">
         <v>89</v>
       </c>
-      <c r="F80">
+      <c r="F80" t="s">
+        <v>245</v>
+      </c>
+      <c r="G80" t="s">
+        <v>89</v>
+      </c>
+      <c r="H80">
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>84</v>
       </c>
@@ -2640,11 +3215,17 @@
       <c r="E81" t="s">
         <v>89</v>
       </c>
-      <c r="F81">
+      <c r="F81" t="s">
+        <v>165</v>
+      </c>
+      <c r="G81" t="s">
+        <v>89</v>
+      </c>
+      <c r="H81">
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -2660,11 +3241,17 @@
       <c r="E82" t="s">
         <v>89</v>
       </c>
-      <c r="F82">
+      <c r="F82" t="s">
+        <v>246</v>
+      </c>
+      <c r="G82" t="s">
+        <v>89</v>
+      </c>
+      <c r="H82">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>86</v>
       </c>
@@ -2680,11 +3267,17 @@
       <c r="E83" t="s">
         <v>89</v>
       </c>
-      <c r="F83">
+      <c r="F83" t="s">
+        <v>167</v>
+      </c>
+      <c r="G83" t="s">
+        <v>89</v>
+      </c>
+      <c r="H83">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -2700,11 +3293,17 @@
       <c r="E84" t="s">
         <v>91</v>
       </c>
-      <c r="F84">
+      <c r="F84" t="s">
+        <v>247</v>
+      </c>
+      <c r="G84" t="s">
+        <v>90</v>
+      </c>
+      <c r="H84">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -2720,7 +3319,13 @@
       <c r="E85" t="s">
         <v>89</v>
       </c>
-      <c r="F85">
+      <c r="F85" t="s">
+        <v>215</v>
+      </c>
+      <c r="G85" t="s">
+        <v>89</v>
+      </c>
+      <c r="H85">
         <v>9</v>
       </c>
     </row>

</xml_diff>